<commit_message>
Update: gantt & resque- bot.eapx
</commit_message>
<xml_diff>
--- a/gantt.xlsx
+++ b/gantt.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D53965-2CCA-487C-9BAC-3C41536AE427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139D2206-850D-437E-9A1C-6BE4A9794CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15480" yWindow="-3135" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektplan" sheetId="11" r:id="rId1"/>
@@ -1273,6 +1273,28 @@
     <xf numFmtId="171" fontId="10" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="8" fillId="8" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="45" borderId="2" xfId="12" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="45" borderId="2" xfId="11" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="45" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="45" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1283,28 +1305,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="169" fontId="8" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="8" fillId="8" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="45" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="45" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="45" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="45" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1919,7 +1919,7 @@
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1964,117 +1964,117 @@
         <v>40</v>
       </c>
       <c r="B3" s="48"/>
-      <c r="C3" s="82" t="s">
+      <c r="C3" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="83"/>
-      <c r="E3" s="81">
+      <c r="D3" s="84"/>
+      <c r="E3" s="89">
         <v>44025</v>
       </c>
-      <c r="F3" s="81"/>
+      <c r="F3" s="89"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="82" t="s">
+      <c r="C4" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="83"/>
+      <c r="D4" s="84"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="78">
+      <c r="I4" s="86">
         <f>I5</f>
         <v>44025</v>
       </c>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="78">
+      <c r="J4" s="87"/>
+      <c r="K4" s="87"/>
+      <c r="L4" s="87"/>
+      <c r="M4" s="87"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="88"/>
+      <c r="P4" s="86">
         <f>P5</f>
         <v>44032</v>
       </c>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="79"/>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="78">
+      <c r="Q4" s="87"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
+      <c r="T4" s="87"/>
+      <c r="U4" s="87"/>
+      <c r="V4" s="88"/>
+      <c r="W4" s="86">
         <f>W5</f>
         <v>44039</v>
       </c>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="79"/>
-      <c r="Z4" s="79"/>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="80"/>
-      <c r="AD4" s="78">
+      <c r="X4" s="87"/>
+      <c r="Y4" s="87"/>
+      <c r="Z4" s="87"/>
+      <c r="AA4" s="87"/>
+      <c r="AB4" s="87"/>
+      <c r="AC4" s="88"/>
+      <c r="AD4" s="86">
         <f>AD5</f>
         <v>44046</v>
       </c>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="79"/>
-      <c r="AG4" s="79"/>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="80"/>
-      <c r="AK4" s="78">
+      <c r="AE4" s="87"/>
+      <c r="AF4" s="87"/>
+      <c r="AG4" s="87"/>
+      <c r="AH4" s="87"/>
+      <c r="AI4" s="87"/>
+      <c r="AJ4" s="88"/>
+      <c r="AK4" s="86">
         <f>AK5</f>
         <v>44053</v>
       </c>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="79"/>
-      <c r="AN4" s="79"/>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="80"/>
-      <c r="AR4" s="78">
+      <c r="AL4" s="87"/>
+      <c r="AM4" s="87"/>
+      <c r="AN4" s="87"/>
+      <c r="AO4" s="87"/>
+      <c r="AP4" s="87"/>
+      <c r="AQ4" s="88"/>
+      <c r="AR4" s="86">
         <f>AR5</f>
         <v>44060</v>
       </c>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="79"/>
-      <c r="AU4" s="79"/>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="80"/>
-      <c r="AY4" s="78">
+      <c r="AS4" s="87"/>
+      <c r="AT4" s="87"/>
+      <c r="AU4" s="87"/>
+      <c r="AV4" s="87"/>
+      <c r="AW4" s="87"/>
+      <c r="AX4" s="88"/>
+      <c r="AY4" s="86">
         <f>AY5</f>
         <v>44067</v>
       </c>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="79"/>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="80"/>
-      <c r="BF4" s="78">
+      <c r="AZ4" s="87"/>
+      <c r="BA4" s="87"/>
+      <c r="BB4" s="87"/>
+      <c r="BC4" s="87"/>
+      <c r="BD4" s="87"/>
+      <c r="BE4" s="88"/>
+      <c r="BF4" s="86">
         <f>BF5</f>
         <v>44074</v>
       </c>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="79"/>
-      <c r="BI4" s="79"/>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="80"/>
+      <c r="BG4" s="87"/>
+      <c r="BH4" s="87"/>
+      <c r="BI4" s="87"/>
+      <c r="BJ4" s="87"/>
+      <c r="BK4" s="87"/>
+      <c r="BL4" s="88"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="85"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
       <c r="I5" s="75">
         <f>_xlfn.SINGLE(Projekt_Start)-WEEKDAY(_xlfn.SINGLE(Projekt_Start),1)+2+7*(_xlfn.SINGLE(Woche_anzeigen)-1)</f>
         <v>44025</v>
@@ -2625,19 +2625,19 @@
       <c r="C8" s="49"/>
       <c r="D8" s="15">
         <f>SUM(D9:D13)/5</f>
-        <v>0.1</v>
-      </c>
-      <c r="E8" s="85">
-        <f>_xlfn.SINGLE(Projekt_Start)</f>
+        <v>0.4</v>
+      </c>
+      <c r="E8" s="78">
+        <f t="shared" ref="E8:E13" si="5">_xlfn.SINGLE(Projekt_Start)</f>
         <v>44025</v>
       </c>
-      <c r="F8" s="85">
+      <c r="F8" s="78">
         <f>E8+7</f>
         <v>44032</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13">
-        <f t="shared" ref="H8:H33" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H33" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v>8</v>
       </c>
       <c r="I8" s="29"/>
@@ -2711,16 +2711,16 @@
         <v>0.5</v>
       </c>
       <c r="E9" s="64">
-        <f>_xlfn.SINGLE(Projekt_Start)</f>
+        <f t="shared" si="5"/>
         <v>44025</v>
       </c>
-      <c r="F9" s="85">
+      <c r="F9" s="78">
         <f>E9+6</f>
         <v>44031</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I9" s="29"/>
@@ -2794,16 +2794,16 @@
         <v>0</v>
       </c>
       <c r="E10" s="64">
-        <f>_xlfn.SINGLE(Projekt_Start)</f>
+        <f t="shared" si="5"/>
         <v>44025</v>
       </c>
-      <c r="F10" s="85">
-        <f t="shared" ref="F10:F13" si="6">E10+6</f>
+      <c r="F10" s="78">
+        <f t="shared" ref="F10:F13" si="7">E10+6</f>
         <v>44031</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I10" s="29"/>
@@ -2872,19 +2872,19 @@
         <v>51</v>
       </c>
       <c r="D11" s="16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E11" s="64">
-        <f>_xlfn.SINGLE(Projekt_Start)</f>
+        <f t="shared" si="5"/>
         <v>44025</v>
       </c>
-      <c r="F11" s="85">
-        <f t="shared" si="6"/>
+      <c r="F11" s="78">
+        <f t="shared" si="7"/>
         <v>44031</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I11" s="29"/>
@@ -2953,19 +2953,19 @@
         <v>53</v>
       </c>
       <c r="D12" s="16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E12" s="64">
-        <f>_xlfn.SINGLE(Projekt_Start)</f>
+        <f t="shared" si="5"/>
         <v>44025</v>
       </c>
-      <c r="F12" s="85">
-        <f t="shared" si="6"/>
+      <c r="F12" s="78">
+        <f t="shared" si="7"/>
         <v>44031</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I12" s="29"/>
@@ -3034,19 +3034,19 @@
         <v>55</v>
       </c>
       <c r="D13" s="16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E13" s="64">
-        <f>_xlfn.SINGLE(Projekt_Start)</f>
+        <f t="shared" si="5"/>
         <v>44025</v>
       </c>
-      <c r="F13" s="85">
-        <f t="shared" si="6"/>
+      <c r="F13" s="78">
+        <f t="shared" si="7"/>
         <v>44031</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I13" s="29"/>
@@ -3119,7 +3119,7 @@
       <c r="F14" s="66"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I14" s="29"/>
@@ -3198,7 +3198,7 @@
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I15" s="29"/>
@@ -3272,12 +3272,12 @@
         <v>44032</v>
       </c>
       <c r="F16" s="67">
-        <f t="shared" ref="F16:F19" si="7">E16+6</f>
+        <f t="shared" ref="F16:F19" si="8">E16+6</f>
         <v>44038</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I16" s="29"/>
@@ -3351,12 +3351,12 @@
         <v>44032</v>
       </c>
       <c r="F17" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44038</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I17" s="29"/>
@@ -3430,12 +3430,12 @@
         <v>44032</v>
       </c>
       <c r="F18" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44038</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I18" s="29"/>
@@ -3509,12 +3509,12 @@
         <v>44032</v>
       </c>
       <c r="F19" s="67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>44038</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I19" s="29"/>
@@ -3587,7 +3587,7 @@
       <c r="F20" s="69"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I20" s="29"/>
@@ -3666,7 +3666,7 @@
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I21" s="29"/>
@@ -3740,12 +3740,12 @@
         <v>44039</v>
       </c>
       <c r="F22" s="70">
-        <f t="shared" ref="F22:F25" si="8">E22+6</f>
+        <f t="shared" ref="F22:F25" si="9">E22+6</f>
         <v>44045</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I22" s="29"/>
@@ -3819,12 +3819,12 @@
         <v>44039</v>
       </c>
       <c r="F23" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44045</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I23" s="29"/>
@@ -3898,12 +3898,12 @@
         <v>44039</v>
       </c>
       <c r="F24" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44045</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I24" s="29"/>
@@ -3977,12 +3977,12 @@
         <v>44039</v>
       </c>
       <c r="F25" s="70">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>44045</v>
       </c>
       <c r="G25" s="13"/>
       <c r="H25" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="I25" s="29"/>
@@ -4055,7 +4055,7 @@
       <c r="F26" s="72"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I26" s="29"/>
@@ -4134,7 +4134,7 @@
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="I27" s="29"/>
@@ -4208,12 +4208,12 @@
         <v>44046</v>
       </c>
       <c r="F28" s="73">
-        <f t="shared" ref="F28:F31" si="9">E28+14</f>
+        <f t="shared" ref="F28:F31" si="10">E28+14</f>
         <v>44060</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="I28" s="29"/>
@@ -4287,12 +4287,12 @@
         <v>44046</v>
       </c>
       <c r="F29" s="73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44060</v>
       </c>
       <c r="G29" s="13"/>
       <c r="H29" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="I29" s="29"/>
@@ -4366,12 +4366,12 @@
         <v>44046</v>
       </c>
       <c r="F30" s="73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44060</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="I30" s="29"/>
@@ -4445,12 +4445,12 @@
         <v>44046</v>
       </c>
       <c r="F31" s="73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44060</v>
       </c>
       <c r="G31" s="13"/>
       <c r="H31" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>15</v>
       </c>
       <c r="I31" s="29"/>
@@ -4514,18 +4514,18 @@
       <c r="A32" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="86" t="s">
+      <c r="B32" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="87"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="89">
+      <c r="C32" s="80"/>
+      <c r="D32" s="81"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82">
         <v>44067</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I32" s="29"/>
@@ -4598,7 +4598,7 @@
       <c r="F33" s="74"/>
       <c r="G33" s="28"/>
       <c r="H33" s="28" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I33" s="31"/>
@@ -4670,11 +4670,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4682,6 +4677,11 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="14">

</xml_diff>